<commit_message>
Addressable 적용 작업 1차
</commit_message>
<xml_diff>
--- a/Assets/Excels/ItemTable.xlsx
+++ b/Assets/Excels/ItemTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SebamoGameClient\Assets\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SebamoClient\Assets\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B74D18-155C-4526-8814-1CEDC4C8A609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C299ACCE-B1CA-4234-B6D4-C4779AC8985C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShopItemData" sheetId="5" r:id="rId1"/>
@@ -410,30 +410,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sprites/ItemIcon/Costume_B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/ItemIcon/Costume_A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/ItemIcon/Costume_C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/ItemIcon/Face_A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/ItemIcon/Face_B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/ItemIcon/Face_C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>유니티짱 페이스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -446,18 +422,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sprites/ItemIcon/Eye_A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/ItemIcon/Eye_B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/ItemIcon/Eye_C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>유니티짱 눈</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -486,18 +450,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sprites/ItemIcon/Hair_A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/ItemIcon/Hair_B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/ItemIcon/Hair_C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>유니티짱 헤어</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -522,14 +474,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sprites/ItemIcon/Prop_A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/ItemIcon/Prop_B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>핑크 베놈 단검</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -542,24 +486,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sprites/ItemIcon/Acc_A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>YucoAccessory</t>
   </si>
   <si>
     <t>MisakiAccessory</t>
   </si>
   <si>
-    <t>Sprites/ItemIcon/Acc_B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/ItemIcon/Acc_C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>노란 머리띠</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -608,22 +540,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sprites/Profile/Frame_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/Profile/Frame_02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/Profile/Profile_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/Profile/Profile_02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>크리스마스 프레임</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -788,6 +704,90 @@
   </si>
   <si>
     <t>Net</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Profile/Profile_01.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Profile/Profile_02.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Profile/Frame_01.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Profile/Frame_02.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Acc_C.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Acc_B.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Acc_A.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Hair_C.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Hair_B.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Hair_A.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Eye_C.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Eye_B.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Eye_A.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Face_C.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Face_B.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Prop_A.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Prop_B.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Costume_A.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Costume_B.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Costume_C.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/ItemIcon/Face_A.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1262,7 +1262,7 @@
         <v>50000</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1309,7 +1309,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1318,12 +1318,12 @@
         <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1332,12 +1332,12 @@
         <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1346,7 +1346,7 @@
         <v>100</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1580,7 +1580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404A241D-11AA-458B-A9E4-7769CAC77567}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1629,42 +1629,42 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1677,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B12247E9-C6A0-42EC-8B14-015B5DEEB4B9}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1721,7 +1721,7 @@
         <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1729,7 +1729,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
@@ -1749,13 +1749,13 @@
         <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E4">
         <v>1000</v>
@@ -1769,7 +1769,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>163</v>
       </c>
       <c r="C5" t="s">
         <v>62</v>
@@ -1786,7 +1786,7 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
         <v>63</v>
@@ -1803,7 +1803,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>165</v>
       </c>
       <c r="C7" t="s">
         <v>64</v>
@@ -1820,13 +1820,13 @@
         <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E8">
         <v>1000</v>
@@ -1837,13 +1837,13 @@
         <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="E9">
         <v>1000</v>
@@ -1854,13 +1854,13 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="E10">
         <v>1000</v>
@@ -1871,13 +1871,13 @@
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>158</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E11">
         <v>1000</v>
@@ -1888,13 +1888,13 @@
         <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>157</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E12">
         <v>1000</v>
@@ -1905,13 +1905,13 @@
         <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E13">
         <v>1000</v>
@@ -1922,13 +1922,13 @@
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E14">
         <v>1000</v>
@@ -1939,13 +1939,13 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E15">
         <v>1000</v>
@@ -1956,13 +1956,13 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E16">
         <v>1000</v>
@@ -1973,10 +1973,10 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
         <v>56</v>
@@ -1987,16 +1987,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>151</v>
       </c>
       <c r="C18" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="E18">
         <v>1000</v>
@@ -2004,16 +2004,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="C19" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="E19">
         <v>1000</v>
@@ -2021,16 +2021,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="E20">
         <v>1000</v>
@@ -2038,16 +2038,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E21">
         <v>1000</v>
@@ -2055,16 +2055,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B22" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="C22" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="E22">
         <v>1000</v>
@@ -2072,16 +2072,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C23" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="E23">
         <v>1000</v>
@@ -2089,16 +2089,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="D24" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="E24">
         <v>1000</v>
@@ -2106,16 +2106,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="D25" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="E25">
         <v>1000</v>
@@ -2123,16 +2123,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="C26" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="D26" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="E26">
         <v>1000</v>
@@ -2140,16 +2140,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="B27" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="C27" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="D27" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E27">
         <v>1000</v>
@@ -2165,7 +2165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC9D8DF-8F98-4A33-894A-DEBD309AB1D5}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2186,7 +2186,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -2208,7 +2208,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>
@@ -2228,7 +2228,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -2239,30 +2239,30 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="D6" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2296,7 +2296,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2307,10 +2307,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -2318,16 +2318,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2364,12 +2364,12 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2385,7 +2385,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2393,7 +2393,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B6">
         <v>0</v>

</xml_diff>